<commit_message>
Revert "Revert "Revert "5"""
This reverts commit 66bcc33138f3c24457c381e21123ac01a53122aa.
</commit_message>
<xml_diff>
--- a/1.xlsx
+++ b/1.xlsx
@@ -339,10 +339,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -360,11 +360,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>11111111</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>